<commit_message>
This ads1299 have the vref 4.5v. The mistake is SPI design . Having a resistance.
</commit_message>
<xml_diff>
--- a/EEG_V2.1/PCB_Project.xlsx
+++ b/EEG_V2.1/PCB_Project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2018-Task\2018-武大脑箍\Project\epic_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2018-Task\2018-武大脑箍\EEGProject\EEG_V2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959A65B3-EEC9-4CE8-9195-2B03F4E090C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A594F-1A65-4AA1-B7DD-02F80AD0DECD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="10185" xr2:uid="{ABA28443-AFE4-4CAA-BE68-EAF36694E26D}"/>
   </bookViews>
@@ -996,7 +996,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1068,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>